<commit_message>
Added functionality to make basic NRFI table. Fixed various errors as welll.
</commit_message>
<xml_diff>
--- a/MLB Bet Buddy/schedule.xlsx
+++ b/MLB Bet Buddy/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\source\repos\MLB Bet Buddy\MLB Bet Buddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E2283-E02C-49E8-8F9C-1678D941BCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49B6DFA-F31D-4148-A602-9CA7224BEFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3210" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="126">
   <si>
     <t>Game ID</t>
   </si>
@@ -76,448 +76,328 @@
     <t>Wind Speed</t>
   </si>
   <si>
-    <t>07/19/2023</t>
-  </si>
-  <si>
-    <t>12:35 PM</t>
-  </si>
-  <si>
-    <t>1:05 PM</t>
-  </si>
-  <si>
-    <t>1:15 PM</t>
+    <t>10/01/2023</t>
+  </si>
+  <si>
+    <t>3:05 PM</t>
+  </si>
+  <si>
+    <t>12:05 PM</t>
+  </si>
+  <si>
+    <t>12:07 PM</t>
+  </si>
+  <si>
+    <t>3:07 PM</t>
+  </si>
+  <si>
+    <t>3:10 PM</t>
+  </si>
+  <si>
+    <t>12:10 PM</t>
   </si>
   <si>
     <t>1:10 PM</t>
   </si>
   <si>
-    <t>12:37 PM</t>
-  </si>
-  <si>
-    <t>6:40 PM</t>
-  </si>
-  <si>
-    <t>7:07 PM</t>
-  </si>
-  <si>
-    <t>4:07 PM</t>
-  </si>
-  <si>
-    <t>7:10 PM</t>
-  </si>
-  <si>
-    <t>7:20 PM</t>
-  </si>
-  <si>
-    <t>7:05 PM</t>
+    <t>2:10 PM</t>
+  </si>
+  <si>
+    <t>2:15 PM</t>
+  </si>
+  <si>
+    <t>Baltimore Orioles</t>
+  </si>
+  <si>
+    <t>San Francisco Giants</t>
   </si>
   <si>
     <t>Pittsburgh Pirates</t>
   </si>
   <si>
-    <t>Baltimore Orioles</t>
+    <t>Los Angeles Angels</t>
+  </si>
+  <si>
+    <t>Toronto Blue Jays</t>
+  </si>
+  <si>
+    <t>Detroit Tigers</t>
+  </si>
+  <si>
+    <t>Arizona Diamondbacks</t>
+  </si>
+  <si>
+    <t>Seattle Mariners</t>
+  </si>
+  <si>
+    <t>Colorado Rockies</t>
+  </si>
+  <si>
+    <t>New York Mets</t>
+  </si>
+  <si>
+    <t>Atlanta Braves</t>
+  </si>
+  <si>
+    <t>Chicago White Sox</t>
+  </si>
+  <si>
+    <t>Kansas City Royals</t>
+  </si>
+  <si>
+    <t>Milwaukee Brewers</t>
+  </si>
+  <si>
+    <t>St. Louis Cardinals</t>
+  </si>
+  <si>
+    <t>101-61</t>
+  </si>
+  <si>
+    <t>79-83</t>
+  </si>
+  <si>
+    <t>76-86</t>
+  </si>
+  <si>
+    <t>73-89</t>
+  </si>
+  <si>
+    <t>89-73</t>
+  </si>
+  <si>
+    <t>78-84</t>
+  </si>
+  <si>
+    <t>84-78</t>
+  </si>
+  <si>
+    <t>88-74</t>
+  </si>
+  <si>
+    <t>59-103</t>
+  </si>
+  <si>
+    <t>75-87</t>
+  </si>
+  <si>
+    <t>104-58</t>
+  </si>
+  <si>
+    <t>61-101</t>
+  </si>
+  <si>
+    <t>56-106</t>
+  </si>
+  <si>
+    <t>92-70</t>
+  </si>
+  <si>
+    <t>71-91</t>
+  </si>
+  <si>
+    <t>Kyle Bradish</t>
+  </si>
+  <si>
+    <t>Kyle Harrison</t>
+  </si>
+  <si>
+    <t>Andre Jackson</t>
+  </si>
+  <si>
+    <t>Carson Fulmer</t>
+  </si>
+  <si>
+    <t>Wes Parsons</t>
+  </si>
+  <si>
+    <t>Eduardo Rodriguez</t>
+  </si>
+  <si>
+    <t>Kyle Nelson</t>
+  </si>
+  <si>
+    <t>George Kirby</t>
+  </si>
+  <si>
+    <t>Brent Suter</t>
+  </si>
+  <si>
+    <t>José Buttó</t>
+  </si>
+  <si>
+    <t>Dylan Dodd</t>
+  </si>
+  <si>
+    <t>José Ureña</t>
+  </si>
+  <si>
+    <t>Zack Greinke</t>
+  </si>
+  <si>
+    <t>Adrian Houser</t>
+  </si>
+  <si>
+    <t>Miles Mikolas</t>
+  </si>
+  <si>
+    <t>Boston Red Sox</t>
+  </si>
+  <si>
+    <t>Los Angeles Dodgers</t>
+  </si>
+  <si>
+    <t>Miami Marlins</t>
+  </si>
+  <si>
+    <t>Oakland Athletics</t>
+  </si>
+  <si>
+    <t>Tampa Bay Rays</t>
+  </si>
+  <si>
+    <t>Cleveland Guardians</t>
+  </si>
+  <si>
+    <t>Houston Astros</t>
   </si>
   <si>
     <t>Texas Rangers</t>
   </si>
   <si>
-    <t>St. Louis Cardinals</t>
-  </si>
-  <si>
-    <t>Colorado Rockies</t>
-  </si>
-  <si>
-    <t>Oakland Athletics</t>
+    <t>Minnesota Twins</t>
   </si>
   <si>
     <t>Philadelphia Phillies</t>
   </si>
   <si>
-    <t>Toronto Blue Jays</t>
-  </si>
-  <si>
-    <t>Los Angeles Angels</t>
+    <t>Washington Nationals</t>
+  </si>
+  <si>
+    <t>San Diego Padres</t>
+  </si>
+  <si>
+    <t>New York Yankees</t>
+  </si>
+  <si>
+    <t>Chicago Cubs</t>
   </si>
   <si>
     <t>Cincinnati Reds</t>
   </si>
   <si>
-    <t>New York Mets</t>
-  </si>
-  <si>
-    <t>Atlanta Braves</t>
-  </si>
-  <si>
-    <t>Chicago Cubs</t>
-  </si>
-  <si>
-    <t>Kansas City Royals</t>
-  </si>
-  <si>
-    <t>Seattle Mariners</t>
-  </si>
-  <si>
-    <t>(42, 54)</t>
-  </si>
-  <si>
-    <t>(58, 37)</t>
-  </si>
-  <si>
-    <t>(58, 39)</t>
-  </si>
-  <si>
-    <t>(43, 53)</t>
-  </si>
-  <si>
-    <t>(37, 59)</t>
-  </si>
-  <si>
-    <t>(27, 71)</t>
-  </si>
-  <si>
-    <t>(52, 43)</t>
-  </si>
-  <si>
-    <t>(53, 43)</t>
-  </si>
-  <si>
-    <t>(49, 48)</t>
-  </si>
-  <si>
-    <t>(51, 46)</t>
-  </si>
-  <si>
-    <t>(45, 50)</t>
-  </si>
-  <si>
-    <t>(61, 33)</t>
-  </si>
-  <si>
-    <t>(28, 69)</t>
-  </si>
-  <si>
-    <t>(47, 48)</t>
-  </si>
-  <si>
-    <t>Rich Hill</t>
-  </si>
-  <si>
-    <t>Dean Kremer</t>
-  </si>
-  <si>
-    <t>Jon Gray</t>
-  </si>
-  <si>
-    <t>Dakota Hudson</t>
-  </si>
-  <si>
-    <t>Austin Gomber</t>
-  </si>
-  <si>
-    <t>Ken Waldichuk</t>
-  </si>
-  <si>
-    <t>Cristopher Sánchez</t>
-  </si>
-  <si>
-    <t>José Berríos</t>
-  </si>
-  <si>
-    <t>Chase Silseth</t>
-  </si>
-  <si>
-    <t>Graham Ashcraft</t>
-  </si>
-  <si>
-    <t>Justin Verlander</t>
-  </si>
-  <si>
-    <t>Charlie Morton</t>
-  </si>
-  <si>
-    <t>Kyle Hendricks</t>
-  </si>
-  <si>
-    <t>Ryan Yarbrough</t>
-  </si>
-  <si>
-    <t>Luis Castillo</t>
-  </si>
-  <si>
-    <t>Cleveland Guardians</t>
-  </si>
-  <si>
-    <t>Los Angeles Dodgers</t>
-  </si>
-  <si>
-    <t>Tampa Bay Rays</t>
-  </si>
-  <si>
-    <t>Miami Marlins</t>
-  </si>
-  <si>
-    <t>Houston Astros</t>
-  </si>
-  <si>
-    <t>Boston Red Sox</t>
-  </si>
-  <si>
-    <t>Milwaukee Brewers</t>
-  </si>
-  <si>
-    <t>San Diego Padres</t>
-  </si>
-  <si>
-    <t>New York Yankees</t>
-  </si>
-  <si>
-    <t>San Francisco Giants</t>
-  </si>
-  <si>
-    <t>Chicago White Sox</t>
-  </si>
-  <si>
-    <t>Arizona Diamondbacks</t>
-  </si>
-  <si>
-    <t>Washington Nationals</t>
-  </si>
-  <si>
-    <t>Detroit Tigers</t>
-  </si>
-  <si>
-    <t>Minnesota Twins</t>
-  </si>
-  <si>
-    <t>(47, 49)</t>
-  </si>
-  <si>
-    <t>(55, 40)</t>
-  </si>
-  <si>
-    <t>(60, 39)</t>
-  </si>
-  <si>
-    <t>(53, 45)</t>
-  </si>
-  <si>
-    <t>(46, 50)</t>
-  </si>
-  <si>
-    <t>(50, 47)</t>
-  </si>
-  <si>
-    <t>(54, 42)</t>
-  </si>
-  <si>
-    <t>(40, 57)</t>
-  </si>
-  <si>
-    <t>(38, 58)</t>
-  </si>
-  <si>
-    <t>(43, 52)</t>
-  </si>
-  <si>
-    <t>Aaron Civale</t>
-  </si>
-  <si>
-    <t>Julio Urías</t>
-  </si>
-  <si>
-    <t>Zack Littell</t>
-  </si>
-  <si>
-    <t>Sandy Alcantara</t>
-  </si>
-  <si>
-    <t>Brandon Bielak</t>
-  </si>
-  <si>
-    <t>Brayan Bello</t>
-  </si>
-  <si>
-    <t>Colin Rea</t>
-  </si>
-  <si>
-    <t>Yu Darvish</t>
-  </si>
-  <si>
-    <t>Carlos Rodón</t>
-  </si>
-  <si>
-    <t>Ross Stripling</t>
-  </si>
-  <si>
-    <t>Touki Toussaint</t>
-  </si>
-  <si>
-    <t>Ryne Nelson</t>
-  </si>
-  <si>
-    <t>Trevor Williams</t>
-  </si>
-  <si>
-    <t>Eduardo Rodriguez</t>
-  </si>
-  <si>
-    <t>Kenta Maeda</t>
+    <t>100-62</t>
+  </si>
+  <si>
+    <t>50-112</t>
+  </si>
+  <si>
+    <t>99-63</t>
+  </si>
+  <si>
+    <t>90-72</t>
+  </si>
+  <si>
+    <t>87-75</t>
+  </si>
+  <si>
+    <t>82-80</t>
+  </si>
+  <si>
+    <t>83-79</t>
+  </si>
+  <si>
+    <t>Tanner Houck</t>
+  </si>
+  <si>
+    <t>Bobby Miller</t>
+  </si>
+  <si>
+    <t>Ryan Weathers</t>
+  </si>
+  <si>
+    <t>JP Sears</t>
+  </si>
+  <si>
+    <t>Jacob Lopez</t>
+  </si>
+  <si>
+    <t>Lucas Giolito</t>
+  </si>
+  <si>
+    <t>Cristian Javier</t>
+  </si>
+  <si>
+    <t>Dane Dunning</t>
+  </si>
+  <si>
+    <t>Bailey Ober</t>
+  </si>
+  <si>
+    <t>Matt Strahm</t>
+  </si>
+  <si>
+    <t>Jackson Rutledge</t>
+  </si>
+  <si>
+    <t>Pedro Avila</t>
+  </si>
+  <si>
+    <t>Michael King</t>
+  </si>
+  <si>
+    <t>Drew Smyly</t>
+  </si>
+  <si>
+    <t>Hunter Greene</t>
+  </si>
+  <si>
+    <t>Oriole Park at Camden Yards</t>
+  </si>
+  <si>
+    <t>Oracle Park</t>
   </si>
   <si>
     <t>PNC Park</t>
   </si>
   <si>
-    <t>Oriole Park at Camden Yards</t>
-  </si>
-  <si>
-    <t>Globe Life Field</t>
+    <t>Angel Stadium</t>
+  </si>
+  <si>
+    <t>Rogers Centre</t>
+  </si>
+  <si>
+    <t>Comerica Park</t>
+  </si>
+  <si>
+    <t>Chase Field</t>
+  </si>
+  <si>
+    <t>T-Mobile Park</t>
+  </si>
+  <si>
+    <t>Coors Field</t>
+  </si>
+  <si>
+    <t>Citi Field</t>
+  </si>
+  <si>
+    <t>Truist Park</t>
+  </si>
+  <si>
+    <t>Guaranteed Rate Field</t>
+  </si>
+  <si>
+    <t>Kauffman Stadium</t>
+  </si>
+  <si>
+    <t>American Family Field</t>
   </si>
   <si>
     <t>Busch Stadium</t>
   </si>
   <si>
-    <t>Coors Field</t>
-  </si>
-  <si>
-    <t>Oakland Coliseum</t>
-  </si>
-  <si>
-    <t>Citizens Bank Park</t>
-  </si>
-  <si>
-    <t>Rogers Centre</t>
-  </si>
-  <si>
-    <t>Angel Stadium</t>
-  </si>
-  <si>
-    <t>Great American Ball Park</t>
-  </si>
-  <si>
-    <t>Citi Field</t>
-  </si>
-  <si>
-    <t>Truist Park</t>
-  </si>
-  <si>
-    <t>Wrigley Field</t>
-  </si>
-  <si>
-    <t>Kauffman Stadium</t>
-  </si>
-  <si>
-    <t>T-Mobile Park</t>
-  </si>
-  <si>
-    <t>Sunny</t>
-  </si>
-  <si>
-    <t>Partly Cloudy</t>
-  </si>
-  <si>
-    <t>Cloudy</t>
-  </si>
-  <si>
-    <t>Partly cloudy</t>
-  </si>
-  <si>
-    <t>Clear</t>
-  </si>
-  <si>
-    <t>Patchy rain nearby</t>
-  </si>
-  <si>
-    <t>Overcast</t>
-  </si>
-  <si>
-    <t>Heavy snow</t>
-  </si>
-  <si>
-    <t>64.9 °F</t>
-  </si>
-  <si>
-    <t>59.4 °F</t>
-  </si>
-  <si>
-    <t>76.0 °F</t>
-  </si>
-  <si>
-    <t>71.7 °F</t>
-  </si>
-  <si>
-    <t>45.6 °F</t>
-  </si>
-  <si>
-    <t>55.0 °F</t>
-  </si>
-  <si>
-    <t>56.0 °F</t>
-  </si>
-  <si>
-    <t>47.4 °F</t>
-  </si>
-  <si>
-    <t>61.8 °F</t>
-  </si>
-  <si>
-    <t>50.5 °F</t>
-  </si>
-  <si>
-    <t>69.3 °F</t>
-  </si>
-  <si>
-    <t>63.6 °F</t>
-  </si>
-  <si>
-    <t>53.6 °F</t>
-  </si>
-  <si>
-    <t>37.0 °F</t>
-  </si>
-  <si>
-    <t>6.0 mph</t>
-  </si>
-  <si>
-    <t>5.6 mph</t>
-  </si>
-  <si>
-    <t>11.6 mph</t>
-  </si>
-  <si>
-    <t>16.8 mph</t>
-  </si>
-  <si>
-    <t>6.9 mph</t>
-  </si>
-  <si>
-    <t>2.2 mph</t>
-  </si>
-  <si>
-    <t>10.1 mph</t>
-  </si>
-  <si>
-    <t>4.5 mph</t>
-  </si>
-  <si>
-    <t>11.4 mph</t>
-  </si>
-  <si>
-    <t>6.3 mph</t>
-  </si>
-  <si>
-    <t>10.7 mph</t>
-  </si>
-  <si>
-    <t>7.2 mph</t>
-  </si>
-  <si>
-    <t>13.0 mph</t>
-  </si>
-  <si>
-    <t>14.3 mph</t>
-  </si>
-  <si>
-    <t>3.1 mph</t>
+    <t>TO DO</t>
   </si>
 </sst>
 </file>
@@ -890,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,12 +780,12 @@
     <col min="2" max="2" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -979,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>717348</v>
+        <v>716367</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -988,49 +868,49 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I2" s="2">
-        <v>448179</v>
+        <v>680694</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="2">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N2" s="2">
-        <v>650644</v>
+        <v>656557</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P2" s="2">
         <v>101</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1038,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>717343</v>
+        <v>716363</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
@@ -1047,49 +927,49 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I3" s="2">
-        <v>665152</v>
+        <v>690986</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K3" s="2">
         <v>119</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="N3" s="2">
-        <v>628711</v>
+        <v>676272</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="P3" s="2">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1097,58 +977,58 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>717346</v>
+        <v>716362</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I4" s="2">
-        <v>592351</v>
+        <v>656578</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K4" s="2">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N4" s="2">
+        <v>677960</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="P4" s="2">
         <v>101</v>
       </c>
-      <c r="N4" s="2">
-        <v>641793</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="P4" s="2">
-        <v>102</v>
-      </c>
       <c r="Q4" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1156,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>717351</v>
+        <v>716365</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -1165,49 +1045,49 @@
         <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" s="2">
-        <v>641712</v>
+        <v>608334</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K5" s="2">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="N5" s="2">
-        <v>645261</v>
+        <v>676664</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="P5" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1215,7 +1095,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>717345</v>
+        <v>716357</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -1224,49 +1104,49 @@
         <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" s="2">
-        <v>596295</v>
+        <v>641149</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K6" s="2">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N6" s="2">
-        <v>656232</v>
+        <v>682052</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="P6" s="2">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1274,7 +1154,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>717344</v>
+        <v>716361</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -1283,49 +1163,49 @@
         <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="2">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" s="2">
-        <v>686610</v>
+        <v>593958</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K7" s="2">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="N7" s="2">
-        <v>678394</v>
+        <v>608337</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="P7" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1333,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>717347</v>
+        <v>716358</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
@@ -1342,49 +1222,49 @@
         <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I8" s="2">
-        <v>650911</v>
+        <v>669459</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" s="2">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="N8" s="2">
-        <v>607067</v>
+        <v>664299</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="P8" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1392,58 +1272,58 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>717338</v>
+        <v>716360</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F9" s="2">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" s="2">
-        <v>621244</v>
+        <v>669923</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K9" s="2">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N9" s="2">
-        <v>506433</v>
+        <v>641540</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="P9" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1451,58 +1331,58 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>717339</v>
+        <v>716359</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" s="2">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10" s="2">
-        <v>681217</v>
+        <v>608718</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K10" s="2">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N10" s="2">
-        <v>607074</v>
+        <v>641927</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="P10" s="2">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1510,58 +1390,58 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>717342</v>
+        <v>716355</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" s="2">
-        <v>668933</v>
+        <v>676130</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="2">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="N11" s="2">
-        <v>548389</v>
+        <v>621381</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="P11" s="2">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1569,58 +1449,58 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>717341</v>
+        <v>716354</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" s="2">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12" s="2">
-        <v>434378</v>
+        <v>689266</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" s="2">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N12" s="2">
-        <v>657053</v>
+        <v>671131</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="P12" s="2">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1628,58 +1508,58 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>717340</v>
+        <v>716356</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" s="2">
-        <v>450203</v>
+        <v>570632</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13" s="2">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="N13" s="2">
-        <v>669194</v>
+        <v>658648</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="P13" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1687,58 +1567,58 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>717336</v>
+        <v>716352</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F14" s="2">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>55</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I14" s="2">
-        <v>543294</v>
+        <v>425844</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K14" s="2">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N14" s="2">
-        <v>592866</v>
+        <v>650633</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="P14" s="2">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1746,58 +1626,58 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>717333</v>
+        <v>716364</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F15" s="2">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I15" s="2">
-        <v>642232</v>
+        <v>605288</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K15" s="2">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="N15" s="2">
-        <v>593958</v>
+        <v>592767</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="P15" s="2">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1805,58 +1685,58 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>717335</v>
+        <v>716353</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F16" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I16" s="2">
-        <v>622491</v>
+        <v>571945</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K16" s="2">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N16" s="2">
-        <v>628317</v>
+        <v>668881</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="P16" s="2">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>